<commit_message>
Cập nhật Timesheets.xlsx từ 22-10 tới 28-10
</commit_message>
<xml_diff>
--- a/Documents/Timesheets.xlsx
+++ b/Documents/Timesheets.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minh Phan\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="24-9_30-9" sheetId="1" r:id="rId1"/>
     <sheet name="1-10_7-10" sheetId="2" r:id="rId2"/>
     <sheet name="8-10_14-10" sheetId="3" r:id="rId3"/>
     <sheet name="15-10_21-10" sheetId="5" r:id="rId4"/>
+    <sheet name="22-10_28-10" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="57">
   <si>
     <t>STT</t>
   </si>
@@ -168,6 +164,36 @@
   </si>
   <si>
     <t>Review tài liệu</t>
+  </si>
+  <si>
+    <t>[Front-end] Tìm hiểu framework Laravel và lập trình giao diện chính</t>
+  </si>
+  <si>
+    <t>Review code</t>
+  </si>
+  <si>
+    <t>Tìm hiểu framework Laravel</t>
+  </si>
+  <si>
+    <t>Lên kế hoạch và phân chia công việc</t>
+  </si>
+  <si>
+    <t>[Back-end] Tìm hiểu framework Laravel và lập trình chức năng gửi thông báo</t>
+  </si>
+  <si>
+    <t>[Back-end] Tìm hiểu framework Laravel và lập trình chức năng thêm người quản lý</t>
+  </si>
+  <si>
+    <t>[Back-end] Tìm hiểu framework Laravel và lập trình chức năng đính kèm file</t>
+  </si>
+  <si>
+    <t>[Back-end] Tìm hiểu framework Laravel và lập trình chức năng thêm lớp, sửa thông tin</t>
+  </si>
+  <si>
+    <t>[Back-end] Tìm hiểu framework Laravel và lập trình chức năng gửi lời mời qua Email</t>
+  </si>
+  <si>
+    <t>[Back-end] Tìm hiểu framework Laravel và lập trình chức năng tham gia lớp</t>
   </si>
 </sst>
 </file>
@@ -358,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,7 +419,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,7 +596,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1340,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,4 +1763,319 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="83" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1152003</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12">
+        <v>1012206</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1212393</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>4</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1212040</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1012402</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>6</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1112091</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1212113</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11">
+        <v>8</v>
+      </c>
+      <c r="B18" s="12">
+        <v>1212219</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>9</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1012162</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
+        <v>10</v>
+      </c>
+      <c r="B24" s="12">
+        <v>1212239</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>11</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1212250</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật lại timesheet cho tất cả các thành viên
Cập nhật Timesheet
</commit_message>
<xml_diff>
--- a/Documents/Timesheets.xlsx
+++ b/Documents/Timesheets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="24-9_30-9" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,10 @@
     <sheet name="22-10_28-10" sheetId="6" r:id="rId5"/>
     <sheet name="29-10_4-11" sheetId="7" r:id="rId6"/>
     <sheet name="5-11_12-11" sheetId="8" r:id="rId7"/>
-    <sheet name="13-11_10-12" sheetId="9" r:id="rId8"/>
+    <sheet name="13-11_20-11" sheetId="9" r:id="rId8"/>
+    <sheet name="21-11_28-11" sheetId="10" r:id="rId9"/>
+    <sheet name="29-11_6-12" sheetId="11" r:id="rId10"/>
+    <sheet name="7-12_13-12" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="114">
   <si>
     <t>STT</t>
   </si>
@@ -220,9 +223,6 @@
     <t>[Front-end] Tìm hiểu framework Laravel và lập trình giao diện hệ thống</t>
   </si>
   <si>
-    <t>Xây dựng chức năng chat</t>
-  </si>
-  <si>
     <t>Nguyễn Văn An</t>
   </si>
   <si>
@@ -235,43 +235,142 @@
     <t>Phạm Lưu Thanh Bình</t>
   </si>
   <si>
-    <t>Kết quả kiểm chứng</t>
-  </si>
-  <si>
-    <t>[Back-end] Hoàn thiện chức năng Send announcement</t>
-  </si>
-  <si>
     <t>[Back-end]  Fix bug chức năng chọn lớp</t>
   </si>
   <si>
     <t>Hoàn thiện chức năng Thêm lớp và sửa thông tin</t>
   </si>
   <si>
-    <t>Fix bug lỗi chọn lớp trong phần Sen Annoncement</t>
-  </si>
-  <si>
-    <t>Tài liệu Hướng dẫn sử dụng</t>
-  </si>
-  <si>
     <t>[Back-end] Hoàn thiện chức năng Gởi lời mời</t>
   </si>
   <si>
     <t>Báo cáo đánh giá quy trình đã thực hiện.</t>
   </si>
   <si>
-    <t>Hướng dẫn thiết lập môi trường và biên dịch mã nguồn</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Báo cáo đánh giá sản phẩm thu được.</t>
   </si>
   <si>
-    <t>Báo cáo đánh giá sản phẩm thu được</t>
-  </si>
-  <si>
-    <t>Test lại hệ thống để cập nhât là kết quả kiểm thử</t>
-  </si>
-  <si>
-    <t>Xây dựng fornt-end phần chọn Rule và giao diện  Student and Parents ,giao diện chat</t>
+    <t>Xây dựng chức năng chat (Chọn lớp để chat)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xây dựng fornt-end phần chọn Rule </t>
+  </si>
+  <si>
+    <t>Fix bug lỗi chọn lớp trong phần Send Annoncement</t>
+  </si>
+  <si>
+    <t>Cập nhật tài liệu thiết lập môi trường và biên dịch mã nguồn</t>
+  </si>
+  <si>
+    <t>Việt hóa Trang đăng nhập và đăng ký</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Back-end] Hoàn thiện chức năng Send announcement trên 1 lớp </t>
+  </si>
+  <si>
+    <t>[Back-end]  Xây dựng chức năng chọn lớp</t>
+  </si>
+  <si>
+    <t>Xây dựng chức năng tham gia lớp</t>
+  </si>
+  <si>
+    <t>Xây dựng tài liệu Kết quả kiểm chứng</t>
+  </si>
+  <si>
+    <t>Cập nhật tài liệu Hướng dẫn thiết lập môi trường và biên dịch mã nguồn</t>
+  </si>
+  <si>
+    <t>Xây dựng chức năng chat (Xóa lịch sử chat)</t>
+  </si>
+  <si>
+    <t>Hoàn thiện Báo cáo đánh giá quy trình đã thực hiện.</t>
+  </si>
+  <si>
+    <t>Tạo Tài Liệu Báo cáo đánh giá sản phẩm thu được</t>
+  </si>
+  <si>
+    <t>Việt hóa trang Class và Rule</t>
+  </si>
+  <si>
+    <t>Ghép Back-end với fornt- end</t>
+  </si>
+  <si>
+    <t>Xây dựng Báo cáo đánh giá sản phẩm thu được</t>
+  </si>
+  <si>
+    <t>Tạo Tài liệu Hướng dẫn sử dụng</t>
+  </si>
+  <si>
+    <t>Review tài liệu Báo cáo đánh gia quy trình sản phẩm</t>
+  </si>
+  <si>
+    <t>Xây dựng chức năng gởi thông báo theo giờ</t>
+  </si>
+  <si>
+    <t>[Back-end]  Chức năng xóa User</t>
+  </si>
+  <si>
+    <t>Kiểm tra test trên hệ thống hiện tại</t>
+  </si>
+  <si>
+    <t>Lập Test Report cho tài liệu</t>
+  </si>
+  <si>
+    <t>[Back-end] Hoàn thành chức năng tham gia lớp</t>
+  </si>
+  <si>
+    <t>Hiện thi danh sách các lớp tham gia</t>
+  </si>
+  <si>
+    <t>Fix lỗi và hoàn thiện chức năng Chat</t>
+  </si>
+  <si>
+    <t>Review lại các tài liệu</t>
+  </si>
+  <si>
+    <t>Xây dựng tài liệu Phát biều công việc</t>
+  </si>
+  <si>
+    <t>Quản lý và phân công công việc của từng thành viên</t>
+  </si>
+  <si>
+    <t>Test chức năng trên các hệ thống hiện tại và thông báo bug tới các thành viên</t>
+  </si>
+  <si>
+    <t>Xây dựng chức năng Send Annocenment trên nhiều lớp</t>
+  </si>
+  <si>
+    <t>Phân quyền cho từng loại tài khoản trong chức năng Send Annoncement</t>
+  </si>
+  <si>
+    <t>[Back-end]  Chức năng thay đổi thông tin tài khoản và mật khẩu</t>
+  </si>
+  <si>
+    <t>Xây dựng fornt-end phần chọn Student</t>
+  </si>
+  <si>
+    <t>Xây dựng fornt-end phần chọn Parent và Setting</t>
+  </si>
+  <si>
+    <t>Hiện thi danh sách các thành viên trong lớp</t>
+  </si>
+  <si>
+    <t>Kiểm tra test trên hệ thống hiện tại lần 2</t>
+  </si>
+  <si>
+    <t>Kiểm tra lại cầu trúc code trong mã nguồn</t>
+  </si>
+  <si>
+    <t>Kiểm tra giao diện hệ thống</t>
+  </si>
+  <si>
+    <t>Fix lỗi còn tồn tại trong hệ thống</t>
+  </si>
+  <si>
+    <t>Kiểm tra test trên hệ thống hiện tại lần cuối</t>
+  </si>
+  <si>
+    <t>Hoàn thiên sản phẩm</t>
   </si>
 </sst>
 </file>
@@ -372,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -413,6 +512,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,7 +793,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -881,6 +989,811 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D45" sqref="A1:D45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="85.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1152003</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1012206</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1212393</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>4</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1212014</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1012402</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11">
+        <v>6</v>
+      </c>
+      <c r="B18" s="12">
+        <v>1212067</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>7</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1212113</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>8</v>
+      </c>
+      <c r="B27" s="12">
+        <v>1212219</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>9</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1012162</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11">
+        <v>10</v>
+      </c>
+      <c r="B37" s="12">
+        <v>1212239</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="11"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>11</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1212250</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4">
+        <v>1212024</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="107.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1152003</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1012206</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1212393</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>4</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1212014</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1012402</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11">
+        <v>6</v>
+      </c>
+      <c r="B16" s="12">
+        <v>1212067</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>7</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1212113</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
+        <v>8</v>
+      </c>
+      <c r="B21" s="12">
+        <v>1212219</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1012162</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11">
+        <v>10</v>
+      </c>
+      <c r="B26" s="12">
+        <v>1212239</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>11</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1212250</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>12</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1212024</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
@@ -2173,7 +3086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -2476,8 +3389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="A1:D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,10 +3701,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="A1:D33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,7 +3714,7 @@
     <col min="4" max="4" width="88.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2826,7 +3739,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2834,7 +3747,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2856,7 +3769,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2864,123 +3777,443 @@
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
       <c r="D6" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1212393</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>4</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1212014</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1012402</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>6</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1212067</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1212113</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
+        <v>8</v>
+      </c>
+      <c r="B17" s="12">
+        <v>1212219</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>79</v>
       </c>
     </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>9</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1012162</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
+        <v>10</v>
+      </c>
+      <c r="B23" s="12">
+        <v>1212239</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>11</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1212250</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4">
+        <v>1212024</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="68.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1152003</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12">
+        <v>1012206</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="11" t="s">
-        <v>46</v>
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1212393</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1212393</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="17" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="17" t="s">
-        <v>58</v>
+      <c r="A9" s="11">
+        <v>4</v>
+      </c>
+      <c r="B9" s="12">
+        <v>1212014</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
-        <v>4</v>
-      </c>
-      <c r="B10" s="12">
-        <v>1212014</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1012402</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>6</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1212067</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>5</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1012402</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
-        <v>6</v>
-      </c>
-      <c r="B14" s="12">
-        <v>1212067</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>67</v>
-      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11" t="s">
-        <v>74</v>
+      <c r="A16" s="4">
+        <v>7</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1212113</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>7</v>
-      </c>
-      <c r="B17" s="5">
-        <v>1212113</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="4" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2988,29 +4221,29 @@
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
       <c r="D18" s="4" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="4" t="s">
-        <v>48</v>
+      <c r="A19" s="11">
+        <v>8</v>
+      </c>
+      <c r="B19" s="12">
+        <v>1212219</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
-        <v>8</v>
-      </c>
-      <c r="B20" s="12">
-        <v>1212219</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="11" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3018,29 +4251,29 @@
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
       <c r="D21" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="11" t="s">
+      <c r="A22" s="4">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1012162</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
-        <v>9</v>
-      </c>
-      <c r="B23" s="5">
-        <v>1012162</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="4" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3048,7 +4281,7 @@
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="4" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3056,85 +4289,76 @@
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
       <c r="D25" s="4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="4" t="s">
+      <c r="A26" s="11">
+        <v>10</v>
+      </c>
+      <c r="B26" s="12">
+        <v>1212239</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>11</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1212250</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4">
+        <v>1212024</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
-        <v>10</v>
-      </c>
-      <c r="B27" s="12">
-        <v>1212239</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
-        <v>11</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1212250</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4">
-        <v>1212024</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D32" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="4" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>